<commit_message>
Adding and improving the debug and console table
</commit_message>
<xml_diff>
--- a/ObjetivosSemanais.xlsx
+++ b/ObjetivosSemanais.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\TCC\emulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{499803B5-2747-40DF-9A10-6E155A488C38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5D380F8-9E7D-4F4E-9454-8B514D2E7034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{92F175DB-81AB-4D87-89D6-10835D3F33E0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Visual Similar a IDE</t>
   </si>
@@ -69,6 +69,15 @@
   </si>
   <si>
     <t>Titulo do arquivo</t>
+  </si>
+  <si>
+    <t>Melhorar lista de abas</t>
+  </si>
+  <si>
+    <t>Ao invés de Texto, grid de tabela</t>
+  </si>
+  <si>
+    <t>mostrar a linha pausada</t>
   </si>
 </sst>
 </file>
@@ -449,7 +458,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,7 +573,9 @@
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
+      <c r="E9" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
@@ -574,7 +585,9 @@
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+      <c r="F10" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -584,7 +597,9 @@
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
+      <c r="G11" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>

</xml_diff>